<commit_message>
Updated from audio filter bom v2
</commit_message>
<xml_diff>
--- a/hardware/audio filter.xlsx
+++ b/hardware/audio filter.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phiphase.RUBIDIUM\Documents\Amateur Radio\audio filter\audio filter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4667DDE3-2F2D-46AD-BF56-BC7E6AF7BCDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10272FB5-554B-408C-B338-D4C2EE17988A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-390" yWindow="4620" windowWidth="30465" windowHeight="15375" xr2:uid="{B02C30A1-D208-4DBA-BA04-AF7AA710FC17}"/>
+    <workbookView xWindow="4635" yWindow="600" windowWidth="30465" windowHeight="15375" xr2:uid="{B02C30A1-D208-4DBA-BA04-AF7AA710FC17}"/>
   </bookViews>
   <sheets>
     <sheet name="audio filter" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'audio filter'!$A$1:$I$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'audio filter'!$A$1:$L$29</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="129">
   <si>
     <t>Reference</t>
   </si>
@@ -121,9 +121,6 @@
     <t>D7</t>
   </si>
   <si>
-    <t>1N4148WT</t>
-  </si>
-  <si>
     <t>https://www.diodes.com/assets/Datasheets/ds30396.pdf</t>
   </si>
   <si>
@@ -163,9 +160,6 @@
     <t>TestPoint</t>
   </si>
   <si>
-    <t>TR1,TR2,TR3,TR4</t>
-  </si>
-  <si>
     <t>2N2222</t>
   </si>
   <si>
@@ -223,15 +217,6 @@
     <t>R1,R2,R3,R4,R6,R7,R9,R11</t>
   </si>
   <si>
-    <t>RV1,RV2,RV3</t>
-  </si>
-  <si>
-    <t>RV4</t>
-  </si>
-  <si>
-    <t>Chassis mount</t>
-  </si>
-  <si>
     <t>Chassis mount 3.5mm</t>
   </si>
   <si>
@@ -241,9 +226,6 @@
     <t>Conn_01x03_Pin</t>
   </si>
   <si>
-    <t>Trim-pot</t>
-  </si>
-  <si>
     <t>Potentiometer</t>
   </si>
   <si>
@@ -280,12 +262,6 @@
     <t>Mouser</t>
   </si>
   <si>
-    <t>737-SW-T2-1C-A-A2-M1</t>
-  </si>
-  <si>
-    <t>858-P090L02F25BR10K</t>
-  </si>
-  <si>
     <t>3mm, 10 mA</t>
   </si>
   <si>
@@ -298,9 +274,6 @@
     <t>Bowood Electronics</t>
   </si>
   <si>
-    <t>Ferrite Bead</t>
-  </si>
-  <si>
     <t>J2, J3, J5</t>
   </si>
   <si>
@@ -343,15 +316,6 @@
     <t>https://www.mouser.co.uk/datasheet/2/393/bpjf_x_series_cd-2943146.pdf</t>
   </si>
   <si>
-    <t>https://www.mouser.co.uk/datasheet/2/4/sw_t2_1x_a_a2_m1_data_sheet-3396473.pdf</t>
-  </si>
-  <si>
-    <t>Adamtech SW-T2-1C-A-A2-M1</t>
-  </si>
-  <si>
-    <t>https://www.mouser.co.uk/datasheet/2/414/P090-3237102.pdf</t>
-  </si>
-  <si>
     <t>TO92</t>
   </si>
   <si>
@@ -361,18 +325,100 @@
     <t>Stick-on feet</t>
   </si>
   <si>
-    <t>858-P091NEC15BR10K</t>
-  </si>
-  <si>
-    <t>72-ACCKPR1417NLS6</t>
+    <t>TR2,TR3,TR4</t>
+  </si>
+  <si>
+    <t>TR1</t>
+  </si>
+  <si>
+    <t>BS170</t>
+  </si>
+  <si>
+    <t>512-BS170</t>
+  </si>
+  <si>
+    <t>TO-92 N-ch Enh. MOSFET</t>
+  </si>
+  <si>
+    <t>https://www.onsemi.com/products/discrete-power-modules/mosfets/small-signal-mosfets/bs170</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>100k</t>
+  </si>
+  <si>
+    <t>6mm round spacer</t>
+  </si>
+  <si>
+    <t>M3 bolt</t>
+  </si>
+  <si>
+    <t>M3 nut</t>
+  </si>
+  <si>
+    <t>M3 Washer</t>
+  </si>
+  <si>
+    <t>NOB160</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/datasheet/2/4/sw_t3_1a_a_a3_s1_data_sheet-3396620.pdf</t>
+  </si>
+  <si>
+    <t>737-SW-T3-1A-A-A3-S1</t>
+  </si>
+  <si>
+    <t>SPST Sub-min toggle switch</t>
+  </si>
+  <si>
+    <t>1N4148</t>
+  </si>
+  <si>
+    <t>Ordered</t>
+  </si>
+  <si>
+    <t>Total price</t>
+  </si>
+  <si>
+    <t>QTY ordered</t>
+  </si>
+  <si>
+    <t>Chassis mount phono socket</t>
+  </si>
+  <si>
+    <t>Chassis mount 5.5mm/2.1mm DC jack</t>
+  </si>
+  <si>
+    <t>858-P160KNP0QC20B10K</t>
+  </si>
+  <si>
+    <t>RV1,RV2,RV3, RV4</t>
+  </si>
+  <si>
+    <t>FRB102</t>
+  </si>
+  <si>
+    <t>RS Components</t>
+  </si>
+  <si>
+    <t>606-759</t>
+  </si>
+  <si>
+    <t>Pack of 50</t>
+  </si>
+  <si>
+    <t>276-9477</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="169" formatCode="&quot;£&quot;#,##0.000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -851,7 +897,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -861,6 +907,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1217,11 +1271,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66F83B6-8D6B-407A-8B05-76CC49A302A5}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,13 +1284,15 @@
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="31.28515625" customWidth="1"/>
     <col min="4" max="5" width="28.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="8" customWidth="1"/>
-    <col min="8" max="8" width="38" customWidth="1"/>
-    <col min="9" max="9" width="38.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="6" customWidth="1"/>
+    <col min="8" max="9" width="13.5703125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="8" customWidth="1"/>
+    <col min="11" max="11" width="38" customWidth="1"/>
+    <col min="12" max="12" width="38.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1247,25 +1303,34 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="I1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1276,25 +1341,35 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F2" s="3">
+        <v>72</v>
+      </c>
+      <c r="F2" s="8">
         <v>9.6</v>
       </c>
-      <c r="G2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H2" t="s">
-        <v>80</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="G2" s="6">
+        <v>1</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*G2</f>
+        <v>9.6</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1305,19 +1380,19 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H3" t="s">
-        <v>81</v>
-      </c>
-      <c r="I3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" t="s">
+        <v>75</v>
+      </c>
+      <c r="L3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1328,19 +1403,19 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>79</v>
-      </c>
-      <c r="G4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H4" t="s">
-        <v>80</v>
-      </c>
-      <c r="I4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J4" t="s">
+        <v>53</v>
+      </c>
+      <c r="K4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1351,22 +1426,32 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F5" s="3">
+        <v>73</v>
+      </c>
+      <c r="F5" s="8">
         <v>3.8</v>
       </c>
-      <c r="G5" t="s">
-        <v>54</v>
-      </c>
-      <c r="H5" t="s">
-        <v>80</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="G5" s="6">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3">
+        <f>F5*G5</f>
+        <v>3.8</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" t="s">
+        <v>52</v>
+      </c>
+      <c r="K5" t="s">
+        <v>74</v>
+      </c>
+      <c r="L5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1376,17 +1461,20 @@
       <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="G6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" t="s">
-        <v>80</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="D6" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" t="s">
+        <v>53</v>
+      </c>
+      <c r="K6" t="s">
+        <v>74</v>
+      </c>
+      <c r="L6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1396,17 +1484,17 @@
       <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="G7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H7" t="s">
-        <v>82</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
+        <v>53</v>
+      </c>
+      <c r="K7" t="s">
+        <v>76</v>
+      </c>
+      <c r="L7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1416,14 +1504,14 @@
       <c r="C8" t="s">
         <v>23</v>
       </c>
-      <c r="G8" t="s">
-        <v>55</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
+        <v>53</v>
+      </c>
+      <c r="L8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1433,14 +1521,14 @@
       <c r="C9" t="s">
         <v>25</v>
       </c>
-      <c r="G9" t="s">
-        <v>55</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
+        <v>53</v>
+      </c>
+      <c r="L9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1450,14 +1538,14 @@
       <c r="C10" t="s">
         <v>27</v>
       </c>
-      <c r="G10" t="s">
-        <v>55</v>
-      </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
+        <v>53</v>
+      </c>
+      <c r="L10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1467,17 +1555,17 @@
       <c r="C11" t="s">
         <v>30</v>
       </c>
-      <c r="G11" t="s">
-        <v>55</v>
-      </c>
-      <c r="H11" t="s">
-        <v>87</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
+        <v>53</v>
+      </c>
+      <c r="K11" t="s">
+        <v>79</v>
+      </c>
+      <c r="L11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -1485,481 +1573,712 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
+        <v>116</v>
+      </c>
+      <c r="J12" t="s">
+        <v>53</v>
+      </c>
+      <c r="L12" t="s">
         <v>32</v>
       </c>
-      <c r="G12" t="s">
-        <v>55</v>
-      </c>
-      <c r="I12" t="s">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>34</v>
       </c>
       <c r="B13">
         <v>6</v>
       </c>
       <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F13" s="8">
+        <v>0.18</v>
+      </c>
+      <c r="G13" s="6">
+        <v>10</v>
+      </c>
+      <c r="H13" s="3">
+        <f>G13*F13</f>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J13" t="s">
+        <v>52</v>
+      </c>
+      <c r="L13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>35</v>
       </c>
-      <c r="D13" t="s">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" t="s">
+        <v>89</v>
+      </c>
+      <c r="F14" s="8">
+        <v>3</v>
+      </c>
+      <c r="G14" s="6">
+        <v>2</v>
+      </c>
+      <c r="H14" s="3">
+        <f>F14*G14</f>
+        <v>6</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J14" t="s">
+        <v>52</v>
+      </c>
+      <c r="K14" t="s">
+        <v>121</v>
+      </c>
+      <c r="L14" t="s">
         <v>90</v>
       </c>
-      <c r="E13" t="s">
-        <v>91</v>
-      </c>
-      <c r="G13" t="s">
-        <v>54</v>
-      </c>
-      <c r="I13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>104</v>
-      </c>
-      <c r="D14" t="s">
-        <v>84</v>
-      </c>
-      <c r="E14" t="s">
-        <v>98</v>
-      </c>
-      <c r="G14" t="s">
-        <v>54</v>
-      </c>
-      <c r="H14" t="s">
-        <v>68</v>
-      </c>
-      <c r="I14" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B15">
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" t="s">
         <v>84</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" s="8">
+        <v>1.85</v>
+      </c>
+      <c r="G15" s="6">
+        <v>3</v>
+      </c>
+      <c r="H15" s="3">
+        <f>F15*G15</f>
+        <v>5.5500000000000007</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J15" t="s">
+        <v>52</v>
+      </c>
+      <c r="K15" t="s">
+        <v>64</v>
+      </c>
+      <c r="L15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" t="s">
+        <v>86</v>
+      </c>
+      <c r="F16" s="8">
+        <v>2.85</v>
+      </c>
+      <c r="G16" s="6">
+        <v>2</v>
+      </c>
+      <c r="H16" s="3">
+        <f>F16*G16</f>
+        <v>5.7</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J16" t="s">
+        <v>52</v>
+      </c>
+      <c r="K16" t="s">
+        <v>65</v>
+      </c>
+      <c r="L16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" t="s">
         <v>93</v>
       </c>
-      <c r="G15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H15" t="s">
-        <v>69</v>
-      </c>
-      <c r="I15" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>94</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="F17" s="8">
+        <v>1.73</v>
+      </c>
+      <c r="G17" s="6">
+        <v>4</v>
+      </c>
+      <c r="H17" s="3">
+        <f>F17*G17</f>
+        <v>6.92</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J17" t="s">
+        <v>52</v>
+      </c>
+      <c r="K17" t="s">
+        <v>120</v>
+      </c>
+      <c r="L17" t="s">
         <v>96</v>
       </c>
-      <c r="D16" t="s">
-        <v>84</v>
-      </c>
-      <c r="E16" t="s">
-        <v>95</v>
-      </c>
-      <c r="G16" t="s">
-        <v>54</v>
-      </c>
-      <c r="H16" t="s">
-        <v>70</v>
-      </c>
-      <c r="I16" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    </row>
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>66</v>
+      </c>
+      <c r="J18" t="s">
+        <v>53</v>
+      </c>
+      <c r="L18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>37</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
-        <v>103</v>
-      </c>
-      <c r="D17" t="s">
-        <v>84</v>
-      </c>
-      <c r="E17" t="s">
-        <v>102</v>
-      </c>
-      <c r="G17" t="s">
-        <v>54</v>
-      </c>
-      <c r="H17" t="s">
-        <v>68</v>
-      </c>
-      <c r="I17" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>64</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>71</v>
-      </c>
-      <c r="G18" t="s">
-        <v>55</v>
-      </c>
-      <c r="I18" t="s">
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+      <c r="J19" t="s">
+        <v>53</v>
+      </c>
+      <c r="L19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G19" t="s">
-        <v>55</v>
-      </c>
-      <c r="I19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B20">
         <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
-      </c>
-      <c r="G20" t="s">
-        <v>55</v>
-      </c>
-      <c r="H20" t="s">
-        <v>74</v>
-      </c>
-      <c r="I20" t="s">
+        <v>39</v>
+      </c>
+      <c r="J20" t="s">
+        <v>53</v>
+      </c>
+      <c r="K20" t="s">
+        <v>68</v>
+      </c>
+      <c r="L20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>123</v>
       </c>
       <c r="B21">
         <v>3</v>
       </c>
       <c r="C21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" t="s">
+        <v>122</v>
+      </c>
+      <c r="F21" s="8">
+        <v>1.37</v>
+      </c>
+      <c r="G21" s="6">
+        <v>4</v>
+      </c>
+      <c r="H21" s="3">
+        <f>F21*G21</f>
+        <v>5.48</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J21" t="s">
+        <v>52</v>
+      </c>
+      <c r="K21" t="s">
+        <v>67</v>
+      </c>
+      <c r="L21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>40</v>
       </c>
-      <c r="D21" t="s">
-        <v>84</v>
-      </c>
-      <c r="E21" t="s">
-        <v>112</v>
-      </c>
-      <c r="G21" t="s">
-        <v>54</v>
-      </c>
-      <c r="H21" t="s">
-        <v>73</v>
-      </c>
-      <c r="I21" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>67</v>
-      </c>
       <c r="B22">
         <v>1</v>
       </c>
-      <c r="C22" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" t="s">
-        <v>84</v>
-      </c>
-      <c r="E22" t="s">
-        <v>86</v>
-      </c>
-      <c r="G22" t="s">
-        <v>54</v>
-      </c>
-      <c r="H22" t="s">
-        <v>72</v>
-      </c>
-      <c r="I22" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>560</v>
+      </c>
+      <c r="J22" t="s">
+        <v>53</v>
+      </c>
+      <c r="L22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>41</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C23">
-        <v>560</v>
-      </c>
-      <c r="G23" t="s">
-        <v>55</v>
-      </c>
-      <c r="I23" t="s">
+        <v>330</v>
+      </c>
+      <c r="J23" t="s">
+        <v>53</v>
+      </c>
+      <c r="L23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>107</v>
+      </c>
+      <c r="J24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>42</v>
-      </c>
-      <c r="B24">
-        <v>3</v>
-      </c>
-      <c r="C24">
-        <v>330</v>
-      </c>
-      <c r="G24" t="s">
-        <v>55</v>
-      </c>
-      <c r="I24" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>43</v>
       </c>
       <c r="B25">
         <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="D25" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E25" t="s">
-        <v>85</v>
-      </c>
-      <c r="G25" t="s">
-        <v>54</v>
-      </c>
-      <c r="H25" t="s">
-        <v>68</v>
-      </c>
-      <c r="I25" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+      <c r="F25" s="8">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="G25" s="6">
+        <v>6</v>
+      </c>
+      <c r="H25" s="3">
+        <f>G25*F25</f>
+        <v>4.3019999999999996</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J25" t="s">
+        <v>52</v>
+      </c>
+      <c r="L25" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B26">
         <v>12</v>
       </c>
       <c r="C26" t="s">
+        <v>44</v>
+      </c>
+      <c r="J26" t="s">
+        <v>53</v>
+      </c>
+      <c r="L26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>101</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>102</v>
+      </c>
+      <c r="D27" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" t="s">
+        <v>103</v>
+      </c>
+      <c r="F27" s="8">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="G27" s="6">
+        <v>10</v>
+      </c>
+      <c r="H27" s="3">
+        <f>G27*F27</f>
+        <v>1.33</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J27" t="s">
+        <v>52</v>
+      </c>
+      <c r="K27" t="s">
+        <v>104</v>
+      </c>
+      <c r="L27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
         <v>45</v>
       </c>
-      <c r="G26" t="s">
+      <c r="D28" t="s">
+        <v>78</v>
+      </c>
+      <c r="E28" t="s">
+        <v>80</v>
+      </c>
+      <c r="F28" s="8">
+        <v>9.4E-2</v>
+      </c>
+      <c r="G28" s="6">
+        <v>50</v>
+      </c>
+      <c r="H28" s="3">
+        <f>G28*F28</f>
+        <v>4.7</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J28" t="s">
+        <v>52</v>
+      </c>
+      <c r="K28" t="s">
+        <v>97</v>
+      </c>
+      <c r="L28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" t="s">
+        <v>78</v>
+      </c>
+      <c r="E29" t="s">
+        <v>81</v>
+      </c>
+      <c r="F29" s="8">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="G29" s="6">
+        <v>1</v>
+      </c>
+      <c r="H29" s="3">
+        <f>G29*F29</f>
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J29" t="s">
+        <v>52</v>
+      </c>
+      <c r="K29" t="s">
+        <v>98</v>
+      </c>
+      <c r="L29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>55</v>
       </c>
-      <c r="I26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>46</v>
-      </c>
-      <c r="B27">
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="J32" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="J33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="J34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="J35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="D36" t="s">
+        <v>82</v>
+      </c>
+      <c r="E36" t="s">
+        <v>112</v>
+      </c>
+      <c r="F36" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G36" s="6">
+        <v>3</v>
+      </c>
+      <c r="H36" s="3">
+        <f>G36*F36</f>
+        <v>1.5</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J36" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37">
+        <v>5</v>
+      </c>
+      <c r="J37" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>99</v>
+      </c>
+      <c r="B38">
         <v>4</v>
       </c>
-      <c r="C27" t="s">
-        <v>47</v>
-      </c>
-      <c r="D27" t="s">
-        <v>84</v>
-      </c>
-      <c r="E27" t="s">
-        <v>88</v>
-      </c>
-      <c r="G27" t="s">
-        <v>54</v>
-      </c>
-      <c r="H27" t="s">
+      <c r="D38" t="s">
+        <v>125</v>
+      </c>
+      <c r="E38" t="s">
+        <v>128</v>
+      </c>
+      <c r="F38" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="G38" s="6">
+        <v>12</v>
+      </c>
+      <c r="H38" s="3">
+        <f>G38*F38</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J38" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>108</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="D39" t="s">
+        <v>125</v>
+      </c>
+      <c r="E39" t="s">
+        <v>126</v>
+      </c>
+      <c r="F39" s="8">
+        <v>7.85</v>
+      </c>
+      <c r="G39" s="6">
+        <v>1</v>
+      </c>
+      <c r="H39" s="3">
+        <v>7.85</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J39" t="s">
+        <v>52</v>
+      </c>
+      <c r="K39" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>109</v>
       </c>
-      <c r="I27" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" t="s">
-        <v>84</v>
-      </c>
-      <c r="E28" t="s">
-        <v>89</v>
-      </c>
-      <c r="G28" t="s">
-        <v>54</v>
-      </c>
-      <c r="H28" t="s">
+      <c r="B40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>110</v>
       </c>
-      <c r="I28" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>57</v>
-      </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="G31" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>59</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="G32" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>60</v>
-      </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="G33" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>61</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="G34" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>62</v>
-      </c>
-      <c r="B35">
-        <v>3</v>
-      </c>
-      <c r="D35" t="s">
-        <v>84</v>
-      </c>
-      <c r="E35" t="s">
-        <v>113</v>
-      </c>
-      <c r="G35" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>63</v>
-      </c>
-      <c r="B36">
-        <v>5</v>
-      </c>
-      <c r="G36" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="B41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>111</v>
       </c>
-      <c r="B37">
+      <c r="B42">
         <v>4</v>
       </c>
-      <c r="G37" t="s">
-        <v>54</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I28" xr:uid="{D66F83B6-8D6B-407A-8B05-76CC49A302A5}">
-    <filterColumn colId="6">
+  <autoFilter ref="A1:L29" xr:uid="{D66F83B6-8D6B-407A-8B05-76CC49A302A5}">
+    <filterColumn colId="9">
       <filters>
         <filter val="No"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{EFD8F6E9-6E2B-4632-B07E-1ADB31C36C3C}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I39" xr:uid="{C259F342-0155-4667-A3CA-003A1B46187C}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1:J1048576" xr:uid="{EFD8F6E9-6E2B-4632-B07E-1ADB31C36C3C}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E21" r:id="rId1" display="https://www.mouser.co.uk/ProductDetail/858-P091N-FC25BR10K" xr:uid="{278AD194-3A37-4245-AEA4-A8C8C6216F9B}"/>
-    <hyperlink ref="E22" r:id="rId2" display="https://www.mouser.co.uk/ProductDetail/858-P090L02F25BR10K" xr:uid="{5ADC1BF8-DE5C-4002-998E-FD6DF70C2DBB}"/>
+    <hyperlink ref="E21" r:id="rId1" display="https://www.mouser.co.uk/ProductDetail/858-P091N-FC25BR10K" xr:uid="{9186C559-F952-449C-8CD6-902719C6B13D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added board layout page.
</commit_message>
<xml_diff>
--- a/hardware/audio filter.xlsx
+++ b/hardware/audio filter.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phiphase.RUBIDIUM\Documents\Amateur Radio\audio filter\audio filter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phiphase\OneDrive\Documents\Amateur Radio\dsp_audio_filter\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10272FB5-554B-408C-B338-D4C2EE17988A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F50A66-2A8D-446A-89D7-D81904ECBE46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4635" yWindow="600" windowWidth="30465" windowHeight="15375" xr2:uid="{B02C30A1-D208-4DBA-BA04-AF7AA710FC17}"/>
+    <workbookView xWindow="7335" yWindow="5835" windowWidth="24150" windowHeight="14085" activeTab="1" xr2:uid="{B02C30A1-D208-4DBA-BA04-AF7AA710FC17}"/>
   </bookViews>
   <sheets>
-    <sheet name="audio filter" sheetId="1" r:id="rId1"/>
+    <sheet name="BOM" sheetId="1" r:id="rId1"/>
+    <sheet name="Connections" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'audio filter'!$A$1:$L$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BOM!$A$1:$L$29</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="161">
   <si>
     <t>Reference</t>
   </si>
@@ -410,6 +411,102 @@
   </si>
   <si>
     <t>276-9477</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>J9</t>
+  </si>
+  <si>
+    <t>J10</t>
+  </si>
+  <si>
+    <t>J11</t>
+  </si>
+  <si>
+    <t>J12</t>
+  </si>
+  <si>
+    <t>KEY_OUT</t>
+  </si>
+  <si>
+    <t>GND</t>
+  </si>
+  <si>
+    <t>AUDIO_IN</t>
+  </si>
+  <si>
+    <t>SPKR+</t>
+  </si>
+  <si>
+    <t>9V</t>
+  </si>
+  <si>
+    <t>HP_OUT</t>
+  </si>
+  <si>
+    <t>TUNE_LED_A</t>
+  </si>
+  <si>
+    <t>PWR_LED_A</t>
+  </si>
+  <si>
+    <t>\TUNE</t>
+  </si>
+  <si>
+    <t>SPKR_AMP_AUDIO_IN</t>
+  </si>
+  <si>
+    <t>\SPKR_ENA</t>
+  </si>
+  <si>
+    <t>SPKR-</t>
+  </si>
+  <si>
+    <t>TUNE_LED_K</t>
+  </si>
+  <si>
+    <t>PWR_LED_K</t>
+  </si>
+  <si>
+    <t>\FC_BW (GND)</t>
+  </si>
+  <si>
+    <t>\FILTER_IN</t>
+  </si>
+  <si>
+    <t>\ALE_IN</t>
+  </si>
+  <si>
+    <t>KEY_IN</t>
+  </si>
+  <si>
+    <t>DOT</t>
+  </si>
+  <si>
+    <t>DASH</t>
+  </si>
+  <si>
+    <t>Pin no.</t>
+  </si>
+  <si>
+    <t>\AN</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
 </sst>
 </file>
@@ -418,7 +515,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
-    <numFmt numFmtId="169" formatCode="&quot;£&quot;#,##0.000"/>
+    <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0.000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -911,10 +1008,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1273,8 +1370,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -2282,4 +2379,237 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50AC2D2B-FDB5-48EE-823D-2B134A5F373B}">
+  <dimension ref="A2:M14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G3" t="s">
+        <v>139</v>
+      </c>
+      <c r="H3" t="s">
+        <v>140</v>
+      </c>
+      <c r="I3" t="s">
+        <v>141</v>
+      </c>
+      <c r="J3" t="s">
+        <v>142</v>
+      </c>
+      <c r="K3" t="s">
+        <v>143</v>
+      </c>
+      <c r="L3" t="s">
+        <v>144</v>
+      </c>
+      <c r="M3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F4" t="s">
+        <v>148</v>
+      </c>
+      <c r="G4" t="s">
+        <v>138</v>
+      </c>
+      <c r="H4" t="s">
+        <v>139</v>
+      </c>
+      <c r="I4" t="s">
+        <v>149</v>
+      </c>
+      <c r="J4" t="s">
+        <v>139</v>
+      </c>
+      <c r="K4" t="s">
+        <v>139</v>
+      </c>
+      <c r="L4" t="s">
+        <v>150</v>
+      </c>
+      <c r="M4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>